<commit_message>
arreglo de letras cortadas
</commit_message>
<xml_diff>
--- a/EmpleadosFirmasTijuana.xlsx
+++ b/EmpleadosFirmasTijuana.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Orlando\Desktop\firmasMasivas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Orlando\Desktop\appFirmas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15C01F7-E371-4D0E-93A6-58AB88B3D6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8946930-6C3D-421A-872F-597162C245BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,21 +219,6 @@
     <t>663 127 7585</t>
   </si>
   <si>
-    <t>L.A.E</t>
-  </si>
-  <si>
-    <t>L.M.I</t>
-  </si>
-  <si>
-    <t>L.C.E.A</t>
-  </si>
-  <si>
-    <t>L.C</t>
-  </si>
-  <si>
-    <t>I.D.I.E</t>
-  </si>
-  <si>
     <t>Rivera Cruz Esteban</t>
   </si>
   <si>
@@ -274,6 +259,21 @@
   </si>
   <si>
     <t>ATN. DEPTO COMERCIAL</t>
+  </si>
+  <si>
+    <t>L.A.E.</t>
+  </si>
+  <si>
+    <t>L.M.I.</t>
+  </si>
+  <si>
+    <t>L.C.E.A.</t>
+  </si>
+  <si>
+    <t>L.C.</t>
+  </si>
+  <si>
+    <t>I.D.I.E.</t>
   </si>
 </sst>
 </file>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,7 +897,7 @@
         <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>34</v>
@@ -929,7 +929,7 @@
         <v>54</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -975,7 +975,7 @@
         <v>55</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
         <v>132</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>30</v>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1010,7 +1010,7 @@
         <v>127</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>24</v>
@@ -1026,10 +1026,10 @@
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>57</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="I7" s="22"/>
     </row>
@@ -1080,7 +1080,7 @@
         <v>58</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="I8" s="22"/>
     </row>
@@ -1133,7 +1133,7 @@
         <v>114</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>28</v>
@@ -1151,7 +1151,7 @@
         <v>60</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="I12" s="22"/>
     </row>
@@ -1224,7 +1224,7 @@
         <v>61</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1232,7 +1232,7 @@
         <v>118</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>24</v>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="22" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
         <v>134</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>29</v>
@@ -1303,10 +1303,10 @@
         <v>142</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>20</v>
@@ -1321,10 +1321,10 @@
         <v>63</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1332,7 +1332,7 @@
         <v>129</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>24</v>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="1" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>